<commit_message>
create two sioux data
</commit_message>
<xml_diff>
--- a/SiouxFallNet/processdata.xlsx
+++ b/SiouxFallNet/processdata.xlsx
@@ -3,22 +3,28 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B4C80A-0943-401B-AB16-4D10D99230C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BC6CF8-B6BC-4B60-8E4B-2B95C5704D86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="2490" windowWidth="17280" windowHeight="9465" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2490" yWindow="2490" windowWidth="17280" windowHeight="9465" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$C$529</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -35,12 +41,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -55,8 +67,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6786,8 +6799,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:C529"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:C510"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B550" sqref="B550"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12610,4 +12623,1235 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E49342-CB41-4D63-8F17-CBB17456BADA}">
+  <dimension ref="A1:D76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <f>A1+1</f>
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <f>B1+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C65" si="0">A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D65" si="1">B2+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>15</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>13</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>12</v>
+      </c>
+      <c r="B38" s="1">
+        <v>11</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>12</v>
+      </c>
+      <c r="B39" s="1">
+        <v>23</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>13</v>
+      </c>
+      <c r="B42">
+        <v>22</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>13</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>18</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>14</v>
+      </c>
+      <c r="B46">
+        <v>21</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>15</v>
+      </c>
+      <c r="B49">
+        <v>16</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>15</v>
+      </c>
+      <c r="B50">
+        <v>17</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>16</v>
+      </c>
+      <c r="B51">
+        <v>9</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>16</v>
+      </c>
+      <c r="B52">
+        <v>15</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>16</v>
+      </c>
+      <c r="B53">
+        <v>18</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>17</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>17</v>
+      </c>
+      <c r="B55">
+        <v>15</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>17</v>
+      </c>
+      <c r="B56">
+        <v>19</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>18</v>
+      </c>
+      <c r="B57">
+        <v>14</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>18</v>
+      </c>
+      <c r="B58">
+        <v>16</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>18</v>
+      </c>
+      <c r="B59">
+        <v>19</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>19</v>
+      </c>
+      <c r="B60">
+        <v>17</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>19</v>
+      </c>
+      <c r="B61">
+        <v>18</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>19</v>
+      </c>
+      <c r="B62">
+        <v>20</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>19</v>
+      </c>
+      <c r="B63">
+        <v>21</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>20</v>
+      </c>
+      <c r="B64">
+        <v>19</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>20</v>
+      </c>
+      <c r="B65">
+        <v>21</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>20</v>
+      </c>
+      <c r="B66">
+        <v>23</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ref="C66:C76" si="2">A66+1</f>
+        <v>21</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ref="D66:D76" si="3">B66+1</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>21</v>
+      </c>
+      <c r="B67">
+        <v>14</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>21</v>
+      </c>
+      <c r="B68">
+        <v>19</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>21</v>
+      </c>
+      <c r="B69">
+        <v>20</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>21</v>
+      </c>
+      <c r="B70">
+        <v>22</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>22</v>
+      </c>
+      <c r="B71">
+        <v>13</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>22</v>
+      </c>
+      <c r="B72">
+        <v>21</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>22</v>
+      </c>
+      <c r="B73">
+        <v>23</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>23</v>
+      </c>
+      <c r="B74">
+        <v>12</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>23</v>
+      </c>
+      <c r="B75">
+        <v>20</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>23</v>
+      </c>
+      <c r="B76">
+        <v>22</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>